<commit_message>
Chnage inpt data in example 16
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/16-PM.Lisa/16-PM.Lisa.xlsx
+++ b/ampl-data-input-excel/16-PM.Lisa/16-PM.Lisa.xlsx
@@ -240,73 +240,73 @@
     <t xml:space="preserve">Work</t>
   </si>
   <si>
+    <t xml:space="preserve">echo.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">echo.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">echo.pm</t>
+    <t xml:space="preserve">foxtrot.pm</t>
   </si>
   <si>
     <t xml:space="preserve">foxtrot.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">foxtrot.pm</t>
+    <t xml:space="preserve">golf.pm</t>
   </si>
   <si>
     <t xml:space="preserve">golf.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">golf.pm</t>
+    <t xml:space="preserve">hotel.pm</t>
   </si>
   <si>
     <t xml:space="preserve">hotel.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">hotel.pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">kilo.pe</t>
   </si>
   <si>
+    <t xml:space="preserve">kilo.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">kilo.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">kilo.pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">lima.pe</t>
   </si>
   <si>
+    <t xml:space="preserve">lima.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">lima.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">lima.pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">whisky2.pe</t>
   </si>
   <si>
+    <t xml:space="preserve">whisky2.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">whisky2.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">whisky2.pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">xray2.pe</t>
   </si>
   <si>
+    <t xml:space="preserve">xray2.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">xray2.pf</t>
   </si>
   <si>
-    <t xml:space="preserve">xray2.pm</t>
-  </si>
-  <si>
     <t xml:space="preserve">zulu2.pe</t>
   </si>
   <si>
+    <t xml:space="preserve">zulu2.pm</t>
+  </si>
+  <si>
     <t xml:space="preserve">zulu2.pf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zulu2.pm</t>
   </si>
   <si>
     <t xml:space="preserve">Expert</t>
@@ -656,6 +656,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -678,10 +682,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -923,7 +923,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="H22:H24 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="H22:H24 C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1029,13 +1029,13 @@
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E1" s="4" t="b">
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="1" sqref="H22:H24 L34"/>
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1691,7 +1691,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="H22:H24 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1729,7 +1729,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="23" t="n">
-        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C614))</f>
+        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C3:C615))</f>
         <v>46002</v>
       </c>
     </row>
@@ -1752,7 +1752,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="H22:H24 F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1811,7 +1811,7 @@
         <f aca="false">misc!A2+1</f>
         <v>45657</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>46002</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -1851,7 +1851,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="H22:H24 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1909,7 +1909,7 @@
         <f aca="false">misc!A2+1</f>
         <v>45657</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>46002</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -1949,7 +1949,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="H22:H24 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2001,7 +2001,7 @@
         <f aca="false">misc!A2+1</f>
         <v>45657</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>46002</v>
       </c>
       <c r="G2" s="5" t="n">
@@ -2038,7 +2038,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="1" sqref="H22:H24 H16"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2109,7 +2109,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H22:H24 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2180,7 +2180,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H22:H24 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2270,8 +2270,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22:H24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2296,15 +2296,15 @@
         <v>6</v>
       </c>
       <c r="E1" s="8" t="b">
-        <f aca="false">AND(E2:E617)</f>
+        <f aca="false">AND(E3:E618)</f>
         <v>1</v>
       </c>
       <c r="F1" s="8" t="b">
-        <f aca="false">AND(F2:F622)</f>
+        <f aca="false">AND(F3:F623)</f>
         <v>1</v>
       </c>
       <c r="G1" s="8" t="b">
-        <f aca="false">AND(G2:G622)</f>
+        <f aca="false">AND(G3:G623)</f>
         <v>1</v>
       </c>
     </row>
@@ -2313,66 +2313,66 @@
         <v>7</v>
       </c>
       <c r="B2" s="9" t="n">
-        <v>45749</v>
+        <v>45658</v>
       </c>
       <c r="C2" s="9" t="n">
-        <v>45794</v>
+        <v>45731</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2" t="b">
         <f aca="false">C2&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2" t="b">
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
-      <c r="H2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="n">
-        <v>45658</v>
+        <v>45749</v>
       </c>
       <c r="C3" s="9" t="n">
-        <v>45731</v>
+        <v>45794</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2" t="b">
         <f aca="false">C3&gt;misc!$A$2</f>
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2" t="b">
         <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
         <v>1</v>
       </c>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="9" t="n">
-        <v>45749</v>
+        <v>45658</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>45779</v>
+        <v>45748</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A4) &gt; 0</f>
@@ -2386,20 +2386,19 @@
         <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
         <v>1</v>
       </c>
-      <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="9" t="n">
-        <v>45658</v>
+        <v>45749</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>45748</v>
+        <v>45779</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A5) &gt; 0</f>
@@ -2413,20 +2412,20 @@
         <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="0"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="9" t="n">
-        <v>45790</v>
+        <v>45658</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>45835</v>
+        <v>45789</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A6) &gt; 0</f>
@@ -2440,20 +2439,20 @@
         <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
         <v>1</v>
       </c>
-      <c r="H6" s="0"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="9" t="n">
-        <v>45658</v>
+        <v>45790</v>
       </c>
       <c r="C7" s="9" t="n">
-        <v>45789</v>
+        <v>45835</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A7) &gt; 0</f>
@@ -2467,20 +2466,20 @@
         <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
         <v>1</v>
       </c>
-      <c r="H7" s="0"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="9" t="n">
-        <v>45902</v>
+        <v>45658</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>45947</v>
+        <v>45901</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E8" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A8) &gt; 0</f>
@@ -2494,20 +2493,20 @@
         <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="0"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="9" t="n">
-        <v>45658</v>
+        <v>45902</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>45901</v>
+        <v>45947</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A9) &gt; 0</f>
@@ -2521,7 +2520,7 @@
         <f aca="false">AND(ISNUMBER(B9), ISNUMBER(C9), B9&lt;=C9)</f>
         <v>1</v>
       </c>
-      <c r="H9" s="0"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -2548,20 +2547,20 @@
         <f aca="false">AND(ISNUMBER(B10), ISNUMBER(C10), B10&lt;=C10)</f>
         <v>1</v>
       </c>
-      <c r="H10" s="0"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="9" t="n">
-        <v>45871</v>
+        <v>45741</v>
       </c>
       <c r="C11" s="9" t="n">
-        <v>45916</v>
+        <v>45870</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E11" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A11) &gt; 0</f>
@@ -2575,20 +2574,20 @@
         <f aca="false">AND(ISNUMBER(B11), ISNUMBER(C11), B11&lt;=C11)</f>
         <v>1</v>
       </c>
-      <c r="H11" s="0"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="9" t="n">
-        <v>45741</v>
+        <v>45871</v>
       </c>
       <c r="C12" s="9" t="n">
-        <v>45870</v>
+        <v>45916</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A12) &gt; 0</f>
@@ -2602,7 +2601,7 @@
         <f aca="false">AND(ISNUMBER(B12), ISNUMBER(C12), B12&lt;=C12)</f>
         <v>1</v>
       </c>
-      <c r="H12" s="0"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -2629,20 +2628,20 @@
         <f aca="false">AND(ISNUMBER(B13), ISNUMBER(C13), B13&lt;=C13)</f>
         <v>1</v>
       </c>
-      <c r="H13" s="0"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="9" t="n">
-        <v>45963</v>
+        <v>45767</v>
       </c>
       <c r="C14" s="9" t="n">
-        <v>45991</v>
+        <v>45962</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A14) &gt; 0</f>
@@ -2656,20 +2655,20 @@
         <f aca="false">AND(ISNUMBER(B14), ISNUMBER(C14), B14&lt;=C14)</f>
         <v>1</v>
       </c>
-      <c r="H14" s="0"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="9" t="n">
-        <v>45767</v>
+        <v>45963</v>
       </c>
       <c r="C15" s="9" t="n">
-        <v>45962</v>
+        <v>45991</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="n">
         <f aca="false">COUNTIF(links!$B$1:$B$562, A15) &gt; 0</f>
@@ -2683,7 +2682,7 @@
         <f aca="false">AND(ISNUMBER(B15), ISNUMBER(C15), B15&lt;=C15)</f>
         <v>1</v>
       </c>
-      <c r="H15" s="0"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -2695,7 +2694,7 @@
       <c r="C16" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
@@ -2719,12 +2718,12 @@
         <v>22</v>
       </c>
       <c r="B17" s="9" t="n">
-        <v>45890</v>
+        <v>45719</v>
       </c>
       <c r="C17" s="9" t="n">
-        <v>45901</v>
-      </c>
-      <c r="D17" s="0" t="n">
+        <v>45889</v>
+      </c>
+      <c r="D17" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="2" t="n">
@@ -2740,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,12 +2747,12 @@
         <v>23</v>
       </c>
       <c r="B18" s="9" t="n">
-        <v>45719</v>
+        <v>45890</v>
       </c>
       <c r="C18" s="9" t="n">
-        <v>45889</v>
-      </c>
-      <c r="D18" s="0" t="n">
+        <v>45901</v>
+      </c>
+      <c r="D18" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
@@ -2769,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,7 +2781,7 @@
       <c r="C19" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="n">
@@ -2806,12 +2805,12 @@
         <v>25</v>
       </c>
       <c r="B20" s="9" t="n">
-        <v>45890</v>
+        <v>45719</v>
       </c>
       <c r="C20" s="9" t="n">
-        <v>45901</v>
-      </c>
-      <c r="D20" s="0" t="n">
+        <v>45889</v>
+      </c>
+      <c r="D20" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
@@ -2827,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,12 +2834,12 @@
         <v>26</v>
       </c>
       <c r="B21" s="9" t="n">
-        <v>45719</v>
+        <v>45890</v>
       </c>
       <c r="C21" s="9" t="n">
-        <v>45889</v>
-      </c>
-      <c r="D21" s="0" t="n">
+        <v>45901</v>
+      </c>
+      <c r="D21" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
@@ -2856,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2868,7 @@
       <c r="C22" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="2" t="n">
@@ -2893,12 +2892,12 @@
         <v>28</v>
       </c>
       <c r="B23" s="9" t="n">
-        <v>45890</v>
+        <v>45719</v>
       </c>
       <c r="C23" s="9" t="n">
-        <v>45901</v>
-      </c>
-      <c r="D23" s="0" t="n">
+        <v>45889</v>
+      </c>
+      <c r="D23" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E23" s="2" t="n">
@@ -2914,7 +2913,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,12 +2921,12 @@
         <v>29</v>
       </c>
       <c r="B24" s="9" t="n">
-        <v>45719</v>
+        <v>45890</v>
       </c>
       <c r="C24" s="9" t="n">
-        <v>45889</v>
-      </c>
-      <c r="D24" s="0" t="n">
+        <v>45901</v>
+      </c>
+      <c r="D24" s="10" t="n">
         <v>0</v>
       </c>
       <c r="E24" s="2" t="n">
@@ -2943,10 +2942,19 @@
         <v>1</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+    </row>
     <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3213,7 +3221,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" error="Planned Go-Live Date must be in the correct date format." errorStyle="stop" errorTitle="Invalid Date" operator="greaterThanOrEqual" prompt=" " promptTitle="Date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C17 C20 C23" type="date">
+    <dataValidation allowBlank="true" error="Planned Go-Live Date must be in the correct date format." errorStyle="stop" errorTitle="Invalid Date" operator="greaterThanOrEqual" prompt=" " promptTitle="Date" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18 C21 C24" type="date">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3241,7 +3249,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="H22:H24 A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3265,7 +3273,7 @@
       </c>
       <c r="D1" s="4" t="b">
         <f aca="false">AND(D2:D627)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3273,14 +3281,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10" t="b">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B2) &gt; 0</f>
+      <c r="D2" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B2) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3289,15 +3297,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="b">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B3) &gt; 0</f>
-        <v>1</v>
+      <c r="D3" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B3) &gt; 0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,14 +3313,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="10" t="b">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B4) &gt; 0</f>
+      <c r="D4" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B4) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3321,14 +3329,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="10" t="b">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B5) &gt; 0</f>
+      <c r="D5" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B5) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3337,14 +3345,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10" t="b">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B6) &gt; 0</f>
+      <c r="D6" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B6) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3353,14 +3361,14 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="10" t="b">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D7" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B7) &gt; 0</f>
+      <c r="D7" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B7) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3369,14 +3377,14 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10" t="b">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B8) &gt; 0</f>
+      <c r="D8" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B8) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3385,14 +3393,14 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10" t="b">
+        <v>13</v>
+      </c>
+      <c r="C9" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D9" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B9) &gt; 0</f>
+      <c r="D9" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B9) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3403,12 +3411,12 @@
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="10" t="b">
+      <c r="C10" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D10" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B10) &gt; 0</f>
+      <c r="D10" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B10) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3417,14 +3425,14 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="10" t="b">
+        <v>17</v>
+      </c>
+      <c r="C11" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D11" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B11) &gt; 0</f>
+      <c r="D11" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B11) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3433,14 +3441,14 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="10" t="b">
+        <v>16</v>
+      </c>
+      <c r="C12" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D12" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B12) &gt; 0</f>
+      <c r="D12" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B12) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3451,12 +3459,12 @@
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="10" t="b">
+      <c r="C13" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D13" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B13) &gt; 0</f>
+      <c r="D13" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B13) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3465,14 +3473,14 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="10" t="b">
+        <v>20</v>
+      </c>
+      <c r="C14" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D14" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B14) &gt; 0</f>
+      <c r="D14" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B14) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3481,14 +3489,14 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="10" t="b">
+        <v>19</v>
+      </c>
+      <c r="C15" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D15" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B15) &gt; 0</f>
+      <c r="D15" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B15) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3499,12 +3507,12 @@
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="10" t="b">
+      <c r="C16" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D16" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B16) &gt; 0</f>
+      <c r="D16" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B16) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3513,14 +3521,14 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="10" t="b">
+        <v>23</v>
+      </c>
+      <c r="C17" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D17" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B17) &gt; 0</f>
+      <c r="D17" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B17) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3529,14 +3537,14 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="10" t="b">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D18" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B18) &gt; 0</f>
+      <c r="D18" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B18) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3547,12 +3555,12 @@
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="10" t="b">
+      <c r="C19" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D19" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B19) &gt; 0</f>
+      <c r="D19" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B19) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3561,14 +3569,14 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="10" t="b">
+        <v>26</v>
+      </c>
+      <c r="C20" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D20" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B20) &gt; 0</f>
+      <c r="D20" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B20) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3577,14 +3585,14 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="10" t="b">
+        <v>25</v>
+      </c>
+      <c r="C21" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D21" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B21) &gt; 0</f>
+      <c r="D21" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B21) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3595,12 +3603,12 @@
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="10" t="b">
+      <c r="C22" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D22" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B22) &gt; 0</f>
+      <c r="D22" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B22) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3609,14 +3617,14 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="10" t="b">
+        <v>29</v>
+      </c>
+      <c r="C23" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A23) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D23" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B23) &gt; 0</f>
+      <c r="D23" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B23) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3625,14 +3633,14 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="10" t="b">
+        <v>28</v>
+      </c>
+      <c r="C24" s="11" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A24) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D24" s="10" t="n">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$617, B24) &gt; 0</f>
+      <c r="D24" s="11" t="n">
+        <f aca="false">COUNTIF(tasks!$A$3:$A$618, B24) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3971,7 +3979,7 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="H22:H24 E22"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3979,7 +3987,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="5" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="12" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="7" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="14" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
@@ -3998,10 +4006,10 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4010,7 +4018,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="9" t="n">
         <v>45749</v>
@@ -4018,10 +4026,10 @@
       <c r="D2" s="9" t="n">
         <v>45794</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="14" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -4030,7 +4038,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>45658</v>
@@ -4038,10 +4046,10 @@
       <c r="D3" s="9" t="n">
         <v>45731</v>
       </c>
-      <c r="E3" s="13" t="n">
+      <c r="E3" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F3" s="13" t="n">
+      <c r="F3" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4050,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>45749</v>
@@ -4058,10 +4066,10 @@
       <c r="D4" s="9" t="n">
         <v>45779</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="14" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -4070,7 +4078,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>45658</v>
@@ -4078,10 +4086,10 @@
       <c r="D5" s="9" t="n">
         <v>45748</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4090,7 +4098,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>45790</v>
@@ -4098,10 +4106,10 @@
       <c r="D6" s="9" t="n">
         <v>45835</v>
       </c>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4110,7 +4118,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>45658</v>
@@ -4118,10 +4126,10 @@
       <c r="D7" s="9" t="n">
         <v>45789</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4130,7 +4138,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>45902</v>
@@ -4138,10 +4146,10 @@
       <c r="D8" s="9" t="n">
         <v>45947</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4150,7 +4158,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>45658</v>
@@ -4158,10 +4166,10 @@
       <c r="D9" s="9" t="n">
         <v>45901</v>
       </c>
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="14" t="n">
         <v>0.25</v>
       </c>
-      <c r="F9" s="13" t="n">
+      <c r="F9" s="14" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -4178,10 +4186,10 @@
       <c r="D10" s="9" t="n">
         <v>45740</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="14" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -4190,7 +4198,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>45871</v>
@@ -4198,10 +4206,10 @@
       <c r="D11" s="9" t="n">
         <v>45916</v>
       </c>
-      <c r="E11" s="13" t="n">
+      <c r="E11" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F11" s="14" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -4210,7 +4218,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>45741</v>
@@ -4218,10 +4226,10 @@
       <c r="D12" s="9" t="n">
         <v>45870</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E12" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F12" s="14" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -4238,10 +4246,10 @@
       <c r="D13" s="9" t="n">
         <v>45766</v>
       </c>
-      <c r="E13" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="n">
+      <c r="E13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="n">
         <v>1.25</v>
       </c>
     </row>
@@ -4250,7 +4258,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>45963</v>
@@ -4258,10 +4266,10 @@
       <c r="D14" s="9" t="n">
         <v>45991</v>
       </c>
-      <c r="E14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="n">
+      <c r="E14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4270,7 +4278,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>45767</v>
@@ -4278,10 +4286,10 @@
       <c r="D15" s="9" t="n">
         <v>45962</v>
       </c>
-      <c r="E15" s="13" t="n">
+      <c r="E15" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="14" t="n">
         <v>0.75</v>
       </c>
     </row>
@@ -4298,10 +4306,10 @@
       <c r="D16" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="E16" s="13" t="n">
+      <c r="E16" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="n">
+      <c r="F16" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4310,7 +4318,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>45890</v>
@@ -4318,10 +4326,10 @@
       <c r="D17" s="9" t="n">
         <v>45901</v>
       </c>
-      <c r="E17" s="13" t="n">
+      <c r="E17" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="13" t="n">
+      <c r="F17" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4330,7 +4338,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="9" t="n">
         <v>45719</v>
@@ -4338,10 +4346,10 @@
       <c r="D18" s="9" t="n">
         <v>45889</v>
       </c>
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="13" t="n">
+      <c r="F18" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4358,10 +4366,10 @@
       <c r="D19" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="E19" s="13" t="n">
+      <c r="E19" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="13" t="n">
+      <c r="F19" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4370,7 +4378,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9" t="n">
         <v>45890</v>
@@ -4378,10 +4386,10 @@
       <c r="D20" s="9" t="n">
         <v>45901</v>
       </c>
-      <c r="E20" s="13" t="n">
+      <c r="E20" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="13" t="n">
+      <c r="F20" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4390,7 +4398,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>45719</v>
@@ -4398,10 +4406,10 @@
       <c r="D21" s="9" t="n">
         <v>45889</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="13" t="n">
+      <c r="F21" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4418,10 +4426,10 @@
       <c r="D22" s="9" t="n">
         <v>45718</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="13" t="n">
+      <c r="F22" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4430,7 +4438,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>45890</v>
@@ -4438,10 +4446,10 @@
       <c r="D23" s="9" t="n">
         <v>45901</v>
       </c>
-      <c r="E23" s="13" t="n">
+      <c r="E23" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="13" t="n">
+      <c r="F23" s="14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -4450,7 +4458,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>45719</v>
@@ -4458,394 +4466,394 @@
       <c r="D24" s="9" t="n">
         <v>45889</v>
       </c>
-      <c r="E24" s="13" t="n">
+      <c r="E24" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="13" t="n">
+      <c r="F24" s="14" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
     </row>
@@ -4982,7 +4990,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H22:H24 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5006,10 +5014,10 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5104,7 +5112,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H22:H24 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5125,308 +5133,308 @@
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
     </row>
     <row r="52" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
     </row>
     <row r="55" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
     </row>
     <row r="64" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
     </row>
     <row r="65" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
     </row>
     <row r="66" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
     </row>
     <row r="67" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
     </row>
     <row r="68" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
     </row>
     <row r="69" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5447,7 +5455,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H22:H24 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5471,32 +5479,32 @@
       <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5581,7 +5589,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H22:H24 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5602,16 +5610,16 @@
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="9"/>
@@ -5780,7 +5788,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="H22:H24 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add caching of loading Excel file
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/16-PM.Lisa/16-PM.Lisa.xlsx
+++ b/ampl-data-input-excel/16-PM.Lisa/16-PM.Lisa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -908,7 +908,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1158,7 +1158,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1256,7 +1256,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1577,7 +1577,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1636,8 +1636,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2615,7 +2615,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="D1" s="4" t="b">
         <f aca="false">AND(D2:D627)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B2) &gt; 0</f>
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B2) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2669,9 +2669,9 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B3) &gt; 0</f>
-        <v>0</v>
+      <c r="D3" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B3) &gt; 0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,8 +2685,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B4) &gt; 0</f>
+      <c r="D4" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B4) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2701,8 +2701,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B5) &gt; 0</f>
+      <c r="D5" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B5) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2717,8 +2717,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D6" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B6) &gt; 0</f>
+      <c r="D6" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B6) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2733,8 +2733,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B7) &gt; 0</f>
+      <c r="D7" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B7) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2749,8 +2749,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B8) &gt; 0</f>
+      <c r="D8" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B8) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2765,8 +2765,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D9" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B9) &gt; 0</f>
+      <c r="D9" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B9) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2781,8 +2781,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B10) &gt; 0</f>
+      <c r="D10" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B10) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2797,8 +2797,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D11" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B11) &gt; 0</f>
+      <c r="D11" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B11) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2813,8 +2813,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D12" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B12) &gt; 0</f>
+      <c r="D12" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B12) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2829,8 +2829,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D13" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B13) &gt; 0</f>
+      <c r="D13" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B13) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2845,8 +2845,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D14" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B14) &gt; 0</f>
+      <c r="D14" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B14) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2861,8 +2861,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D15" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B15) &gt; 0</f>
+      <c r="D15" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B15) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2877,8 +2877,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D16" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B16) &gt; 0</f>
+      <c r="D16" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B16) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2893,8 +2893,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D17" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B17) &gt; 0</f>
+      <c r="D17" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B17) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2909,8 +2909,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D18" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B18) &gt; 0</f>
+      <c r="D18" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B18) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2925,8 +2925,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D19" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B19) &gt; 0</f>
+      <c r="D19" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B19) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2941,8 +2941,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D20" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B20) &gt; 0</f>
+      <c r="D20" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B20) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2957,8 +2957,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D21" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B21) &gt; 0</f>
+      <c r="D21" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B21) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2973,8 +2973,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D22" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B22) &gt; 0</f>
+      <c r="D22" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B22) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -2989,8 +2989,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A23) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D23" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B23) &gt; 0</f>
+      <c r="D23" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B23) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -3005,8 +3005,8 @@
         <f aca="false">COUNTIF(expert!$A$2:$A$954, A24) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="D24" s="11" t="b">
-        <f aca="false">COUNTIF(task!$A$3:$A$618, B24) &gt; 0</f>
+      <c r="D24" s="11" t="n">
+        <f aca="false">COUNTIF(task!$A$2:$A$618, B24) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
@@ -4898,7 +4898,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5264,7 +5264,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5749,8 +5749,8 @@
   </sheetPr>
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>